<commit_message>
fix bugs and sortable
</commit_message>
<xml_diff>
--- a/export.xlsx
+++ b/export.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="111">
   <si>
     <t>To promote the social inclusion and protection of people and families</t>
   </si>
@@ -107,21 +107,6 @@
   </si>
   <si>
     <t>Difference to next</t>
-  </si>
-  <si>
-    <t>teste</t>
-  </si>
-  <si>
-    <t>extreme-very strong</t>
-  </si>
-  <si>
-    <t>weak</t>
-  </si>
-  <si>
-    <t>teste 2</t>
-  </si>
-  <si>
-    <t>very weak</t>
   </si>
   <si>
     <t>upper ref.</t>
@@ -328,6 +313,9 @@
     <t>0</t>
   </si>
   <si>
+    <t>very weak</t>
+  </si>
+  <si>
     <t>very weak - weak</t>
   </si>
   <si>
@@ -341,6 +329,9 @@
   </si>
   <si>
     <t>very weak - extreme</t>
+  </si>
+  <si>
+    <t>weak</t>
   </si>
   <si>
     <t>2</t>
@@ -3198,12 +3189,8 @@
         <f>10000*S16+3000*R16+1000*Q16+200*P16+10*O16+N16-L16-10*K16-200*J16-1000*I16-3000*H16-10000*G16</f>
         <v>0</v>
       </c>
-      <c r="B16" s="66">
-        <v>1.2</v>
-      </c>
-      <c r="C16" s="67" t="s">
-        <v>21</v>
-      </c>
+      <c r="B16" s="66"/>
+      <c r="C16" s="67"/>
       <c r="D16" s="68"/>
       <c r="E16" s="69"/>
       <c r="F16" s="70"/>
@@ -3217,21 +3204,13 @@
       <c r="N16" s="71"/>
       <c r="O16" s="71"/>
       <c r="P16" s="71"/>
-      <c r="Q16" s="71">
-        <v>1</v>
-      </c>
-      <c r="R16" s="71">
-        <v>2</v>
-      </c>
-      <c r="S16" s="71">
-        <v>3</v>
-      </c>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="71"/>
       <c r="T16" s="72"/>
       <c r="U16" s="65"/>
       <c r="V16" s="73"/>
-      <c r="W16" s="74" t="s">
-        <v>22</v>
-      </c>
+      <c r="W16" s="74"/>
       <c r="X16" s="75"/>
       <c r="Y16" s="76"/>
       <c r="Z16" s="77"/>
@@ -3268,19 +3247,13 @@
       <c r="U17" s="65"/>
       <c r="V17" s="73"/>
       <c r="W17" s="74"/>
-      <c r="X17" s="74" t="s">
-        <v>23</v>
-      </c>
+      <c r="X17" s="74"/>
       <c r="Y17" s="73"/>
       <c r="Z17" s="80"/>
       <c r="AA17" s="65"/>
       <c r="AB17" s="71"/>
-      <c r="AC17" s="71">
-        <v>4</v>
-      </c>
-      <c r="AD17" s="71">
-        <v>2</v>
-      </c>
+      <c r="AC17" s="71"/>
+      <c r="AD17" s="71"/>
       <c r="AE17" s="71"/>
       <c r="AF17" s="71"/>
       <c r="AG17" s="71"/>
@@ -3291,25 +3264,15 @@
         <f>10000*S18+3000*R18+1000*Q18+200*P18+10*O18+N18-L18-10*K18-200*J18-1000*I18-3000*H18-10000*G18</f>
         <v>0</v>
       </c>
-      <c r="B18" s="66">
-        <v>1.3</v>
-      </c>
-      <c r="C18" s="67" t="s">
-        <v>24</v>
-      </c>
+      <c r="B18" s="66"/>
+      <c r="C18" s="67"/>
       <c r="D18" s="68"/>
       <c r="E18" s="69"/>
       <c r="F18" s="70"/>
       <c r="G18" s="71"/>
-      <c r="H18" s="71">
-        <v>3</v>
-      </c>
-      <c r="I18" s="71">
-        <v>4</v>
-      </c>
-      <c r="J18" s="71">
-        <v>5</v>
-      </c>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
       <c r="K18" s="71"/>
       <c r="L18" s="71"/>
       <c r="M18" s="71"/>
@@ -3322,9 +3285,7 @@
       <c r="T18" s="72"/>
       <c r="U18" s="65"/>
       <c r="V18" s="73"/>
-      <c r="W18" s="74" t="s">
-        <v>23</v>
-      </c>
+      <c r="W18" s="74"/>
       <c r="X18" s="74"/>
       <c r="Y18" s="73"/>
       <c r="Z18" s="80"/>
@@ -3361,9 +3322,7 @@
       <c r="U19" s="65"/>
       <c r="V19" s="73"/>
       <c r="W19" s="74"/>
-      <c r="X19" s="74" t="s">
-        <v>25</v>
-      </c>
+      <c r="X19" s="74"/>
       <c r="Y19" s="73"/>
       <c r="Z19" s="80"/>
       <c r="AA19" s="65"/>
@@ -3371,15 +3330,9 @@
       <c r="AC19" s="71"/>
       <c r="AD19" s="71"/>
       <c r="AE19" s="71"/>
-      <c r="AF19" s="71">
-        <v>2</v>
-      </c>
-      <c r="AG19" s="71">
-        <v>3</v>
-      </c>
-      <c r="AH19" s="71">
-        <v>1</v>
-      </c>
+      <c r="AF19" s="71"/>
+      <c r="AG19" s="71"/>
+      <c r="AH19" s="71"/>
     </row>
     <row r="20" spans="1:1025" customHeight="1" ht="15">
       <c r="A20" s="65" t="str">
@@ -12129,35 +12082,35 @@
     </row>
     <row r="2" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B2" s="84" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C2"/>
     </row>
     <row r="3" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B3" s="85" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C3"/>
       <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
         <v>28</v>
       </c>
-      <c r="H3" t="s">
+      <c r="M3" t="s">
         <v>29</v>
-      </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:1025" customHeight="1" ht="12.75">
@@ -12167,7 +12120,7 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:1025" customHeight="1" ht="12.75">
@@ -12176,10 +12129,10 @@
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="M5" t="str">
         <f>TRUE()</f>
@@ -12188,23 +12141,23 @@
     </row>
     <row r="6" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B6" s="87" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C6" s="88" t="str">
         <f>C7-1</f>
         <v>0</v>
       </c>
       <c r="D6" s="89" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G6">
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="M6" t="str">
         <f>TRUE()</f>
@@ -12213,23 +12166,23 @@
     </row>
     <row r="7" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B7" s="87" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C7" s="88" t="str">
         <f>C8-1</f>
         <v>0</v>
       </c>
       <c r="D7" s="89" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G7">
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="I7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="M7" t="str">
         <f>TRUE()</f>
@@ -12238,23 +12191,23 @@
     </row>
     <row r="8" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B8" s="87" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C8" s="88" t="str">
         <f>C9-1</f>
         <v>0</v>
       </c>
       <c r="D8" s="89" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G8">
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="M8" t="str">
         <f>TRUE()</f>
@@ -12263,23 +12216,23 @@
     </row>
     <row r="9" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B9" s="87" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C9" s="88" t="str">
         <f>C10-1</f>
         <v>0</v>
       </c>
       <c r="D9" s="89" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G9">
         <v>6</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="I9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="M9" t="str">
         <f>TRUE()</f>
@@ -12288,23 +12241,23 @@
     </row>
     <row r="10" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B10" s="87" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C10" s="88" t="str">
         <f>C11-1</f>
         <v>0</v>
       </c>
       <c r="D10" s="89" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G10">
         <v>7</v>
       </c>
       <c r="H10" s="90" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="M10" t="str">
         <f>TRUE()</f>
@@ -12313,23 +12266,23 @@
     </row>
     <row r="11" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B11" s="87" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C11" s="88" t="str">
         <f>C12-1</f>
         <v>0</v>
       </c>
       <c r="D11" s="89" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G11">
         <v>8</v>
       </c>
       <c r="H11" s="90" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="I11" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="M11" t="str">
         <f>TRUE()</f>
@@ -12338,23 +12291,23 @@
     </row>
     <row r="12" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B12" s="87" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C12" s="88" t="str">
         <f>C13-1</f>
         <v>0</v>
       </c>
       <c r="D12" s="89" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G12">
         <v>9</v>
       </c>
       <c r="H12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="I12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="M12" t="str">
         <f>TRUE()</f>
@@ -12363,139 +12316,139 @@
     </row>
     <row r="13" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B13" s="87" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C13" s="88" t="str">
         <f>C14-1</f>
         <v>0</v>
       </c>
       <c r="D13" s="89" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B14" s="87" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C14" s="88" t="str">
         <f>C15-1</f>
         <v>0</v>
       </c>
       <c r="D14" s="89" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B15" s="87" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C15" s="88" t="str">
         <f>C16-1</f>
         <v>0</v>
       </c>
       <c r="D15" s="89" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B16" s="87" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C16" s="88" t="str">
         <f>C17-1</f>
         <v>0</v>
       </c>
       <c r="D16" s="89" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B17" s="87" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C17" s="88" t="str">
         <f>C18-1</f>
         <v>0</v>
       </c>
       <c r="D17" s="89" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B18" s="87" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C18" s="88" t="str">
         <f>C19-1</f>
         <v>0</v>
       </c>
       <c r="D18" s="89" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B19" s="87" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C19" s="88" t="str">
         <f>C20-1</f>
         <v>0</v>
       </c>
       <c r="D19" s="89" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B20" s="87" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C20" s="88" t="str">
         <f>C21-1</f>
         <v>0</v>
       </c>
       <c r="D20" s="89" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B21" s="87" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C21" s="88" t="str">
         <f>C22-1</f>
         <v>0</v>
       </c>
       <c r="D21" s="89" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B22" s="87" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C22" s="88" t="str">
         <f>C23-1</f>
         <v>0</v>
       </c>
       <c r="D22" s="89" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B23" s="87" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C23" s="88" t="str">
         <f>C24-1</f>
         <v>0</v>
       </c>
       <c r="D23" s="89" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B24" s="87" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C24" s="88" t="str">
         <f>C25-1</f>
@@ -12507,19 +12460,19 @@
     </row>
     <row r="25" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B25" s="87" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C25" s="88" t="str">
         <f>C26-1</f>
         <v>0</v>
       </c>
       <c r="D25" s="91" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B26" s="87" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C26" s="88" t="str">
         <f>C27-1</f>
@@ -12531,18 +12484,18 @@
     </row>
     <row r="27" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B27" s="87" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C27" s="88">
         <v>0</v>
       </c>
       <c r="D27" s="91" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B28" s="87" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="C28" s="88" t="str">
         <f>C27+1</f>
@@ -12554,242 +12507,242 @@
     </row>
     <row r="29" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B29" s="87" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C29" s="88" t="str">
         <f>C28+1</f>
         <v>0</v>
       </c>
       <c r="D29" s="91" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B30" s="87" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C30" s="88" t="str">
         <f>C29+1</f>
         <v>0</v>
       </c>
       <c r="D30" s="91" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B31" s="87" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C31" s="88" t="str">
         <f>C30+1</f>
         <v>0</v>
       </c>
       <c r="D31" s="91" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B32" s="87" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C32" s="88" t="str">
         <f>C31+1</f>
         <v>0</v>
       </c>
       <c r="D32" s="91" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B33" s="87" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C33" s="88" t="str">
         <f>C32+1</f>
         <v>0</v>
       </c>
       <c r="D33" s="91" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B34" s="87" t="s">
-        <v>23</v>
+        <v>95</v>
       </c>
       <c r="C34" s="88" t="str">
         <f>C33+1</f>
         <v>0</v>
       </c>
       <c r="D34" s="91" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B35" s="87" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C35" s="88" t="str">
         <f>C34+1</f>
         <v>0</v>
       </c>
       <c r="D35" s="91" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B36" s="87" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C36" s="88" t="str">
         <f>C35+1</f>
         <v>0</v>
       </c>
       <c r="D36" s="91" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B37" s="87" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C37" s="88" t="str">
         <f>C36+1</f>
         <v>0</v>
       </c>
       <c r="D37" s="91" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B38" s="87" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C38" s="88" t="str">
         <f>C37+1</f>
         <v>0</v>
       </c>
       <c r="D38" s="91" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B39" s="87" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C39" s="88" t="str">
         <f>C38+1</f>
         <v>0</v>
       </c>
       <c r="D39" s="91" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B40" s="87" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C40" s="88" t="str">
         <f>C39+1</f>
         <v>0</v>
       </c>
       <c r="D40" s="91" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B41" s="87" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C41" s="88" t="str">
         <f>C40+1</f>
         <v>0</v>
       </c>
       <c r="D41" s="91" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B42" s="87" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C42" s="88" t="str">
         <f>C41+1</f>
         <v>0</v>
       </c>
       <c r="D42" s="91" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B43" s="87" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C43" s="88" t="str">
         <f>C42+1</f>
         <v>0</v>
       </c>
       <c r="D43" s="91" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B44" s="87" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C44" s="88" t="str">
         <f>C43+1</f>
         <v>0</v>
       </c>
       <c r="D44" s="91" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B45" s="87" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C45" s="88" t="str">
         <f>C44+1</f>
         <v>0</v>
       </c>
       <c r="D45" s="91" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B46" s="87" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C46" s="88" t="str">
         <f>C45+1</f>
         <v>0</v>
       </c>
       <c r="D46" s="91" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B47" s="87" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C47" s="88" t="str">
         <f>C46+1</f>
         <v>0</v>
       </c>
       <c r="D47" s="91" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:1025" customHeight="1" ht="12.75">
       <c r="B48" s="92" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C48" s="93" t="str">
         <f>C47+1</f>
         <v>0</v>
       </c>
       <c r="D48" s="94" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>